<commit_message>
converting juliandate to datetime and datetime to juliandate
</commit_message>
<xml_diff>
--- a/Hand Calc Code Breakdown.xlsx
+++ b/Hand Calc Code Breakdown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rshaf\Documents\Virginia Tech\Spring 2021\AOE 4166\asteroid_orbital_sim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gen's HP\Desktop\Senior Design\asteroid_orbital_sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917C1806-D093-449D-BCC9-AFAA7F860CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0634C263-535C-41E5-9B14-77B1AE7B17FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1B3416D3-5C03-4C79-9DC6-943D6E128DF3}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{1B3416D3-5C03-4C79-9DC6-943D6E128DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="48">
   <si>
     <t>AUXILIARY FUNCTIONS</t>
   </si>
@@ -311,17 +311,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -340,6 +331,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,469 +658,473 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.68359375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5" t="s">
+      <c r="D12" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5" t="s">
+      <c r="D13" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5" t="s">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5" t="s">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11" t="s">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="21" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G26" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="15"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="6" t="s">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="6"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5" t="s">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="1"/>
+      <c r="B30" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="6"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5" t="s">
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="6"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5" t="s">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="6"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="15"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5" t="s">
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="12"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="1"/>
+      <c r="B34" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="6"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11" t="s">
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A35" s="7"/>
+      <c r="B35" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="12"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Made edits to excel file
</commit_message>
<xml_diff>
--- a/Hand Calc Code Breakdown.xlsx
+++ b/Hand Calc Code Breakdown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gen's HP\Desktop\Senior Design\asteroid_orbital_sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0634C263-535C-41E5-9B14-77B1AE7B17FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AD3690-C45C-48DA-B08A-BE7CE6D4B1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{1B3416D3-5C03-4C79-9DC6-943D6E128DF3}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
   <si>
     <t>AUXILIARY FUNCTIONS</t>
   </si>
@@ -176,6 +176,15 @@
   </si>
   <si>
     <t>This may not be needed? Covered by EGA to asteroid plane?</t>
+  </si>
+  <si>
+    <t>juliandate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datetime </t>
+  </si>
+  <si>
+    <t xml:space="preserve">proper syntax in .txt file </t>
   </si>
 </sst>
 </file>
@@ -322,6 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -340,7 +350,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,7 +667,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -672,15 +681,15 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
@@ -830,34 +839,42 @@
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="10" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="10" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1"/>
@@ -867,7 +884,9 @@
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="3"/>
@@ -943,15 +962,15 @@
     </row>
     <row r="21" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="16"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
@@ -1008,15 +1027,15 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1"/>
@@ -1090,15 +1109,15 @@
       <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1"/>

</xml_diff>

<commit_message>
Changes to hand calc breakdown and code structure based on meeting
</commit_message>
<xml_diff>
--- a/Hand Calc Code Breakdown.xlsx
+++ b/Hand Calc Code Breakdown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gen's HP\Desktop\Senior Design\asteroid_orbital_sim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rshaf\Documents\Virginia Tech\Spring 2021\AOE 4166\asteroid_orbital_sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AD3690-C45C-48DA-B08A-BE7CE6D4B1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39F499B-B5AA-4D3D-8B5E-0884F3C50C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{1B3416D3-5C03-4C79-9DC6-943D6E128DF3}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1B3416D3-5C03-4C79-9DC6-943D6E128DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
   <si>
     <t>AUXILIARY FUNCTIONS</t>
   </si>
@@ -40,9 +40,6 @@
     <t xml:space="preserve">Building blocks of trajectory models </t>
   </si>
   <si>
-    <t>Funciton Name</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
     <t>EGA return</t>
   </si>
   <si>
-    <t>This may not be needed? Covered by EGA to asteroid plane?</t>
-  </si>
-  <si>
     <t>juliandate</t>
   </si>
   <si>
@@ -185,6 +179,24 @@
   </si>
   <si>
     <t xml:space="preserve">proper syntax in .txt file </t>
+  </si>
+  <si>
+    <t>Not Needed</t>
+  </si>
+  <si>
+    <t>Covered by EGA to asteroid plane</t>
+  </si>
+  <si>
+    <t>HAND CALC OUTPUT</t>
+  </si>
+  <si>
+    <t>Decide whether to simulate trajectory or discard</t>
+  </si>
+  <si>
+    <t>Function Name</t>
+  </si>
+  <si>
+    <t>Analyze results of hand calculated trajectories</t>
   </si>
 </sst>
 </file>
@@ -320,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -350,6 +362,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,23 +677,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5545043C-77C2-4230-9F1D-CB885AA87625}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -691,7 +704,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -702,7 +715,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -711,259 +724,259 @@
       <c r="F4" s="2"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="21" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -972,9 +985,9 @@
       <c r="F22" s="15"/>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -983,9 +996,9 @@
       <c r="F23" s="2"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -994,7 +1007,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1003,32 +1016,32 @@
       <c r="F25" s="2"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>5</v>
-      </c>
       <c r="E26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -1037,80 +1050,80 @@
       <c r="F27" s="12"/>
       <c r="G27" s="13"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -1119,38 +1132,97 @@
       <c r="F33" s="12"/>
       <c r="G33" s="13"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
     </row>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="16"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+      <c r="B41" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A37:G37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="landscape" horizontalDpi="500" verticalDpi="500" copies="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Outlining changes to excel sheet, again
</commit_message>
<xml_diff>
--- a/Hand Calc Code Breakdown.xlsx
+++ b/Hand Calc Code Breakdown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gen's HP\Desktop\Senior Design\asteroid_orbital_sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AD3690-C45C-48DA-B08A-BE7CE6D4B1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BE944E-9ABA-4586-B72C-E0718763FD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{1B3416D3-5C03-4C79-9DC6-943D6E128DF3}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
   <si>
     <t>AUXILIARY FUNCTIONS</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t xml:space="preserve">proper syntax in .txt file </t>
+  </si>
+  <si>
+    <t>EarthFrame, AsteroidFrame (called from script, E2APatchConic)</t>
   </si>
 </sst>
 </file>
@@ -666,13 +669,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5545043C-77C2-4230-9F1D-CB885AA87625}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="33.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.1015625" customWidth="1"/>
     <col min="2" max="2" width="66.68359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.68359375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.68359375" bestFit="1" customWidth="1"/>
@@ -877,7 +880,9 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="B14" s="2" t="s">
         <v>25</v>
       </c>
@@ -885,7 +890,7 @@
         <v>22</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1103,7 +1108,9 @@
       <c r="C32" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="3"/>

</xml_diff>